<commit_message>
inital macro specification Excel table
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -55,19 +55,19 @@
     <t xml:space="preserve">memory array supply</t>
   </si>
   <si>
-    <t xml:space="preserve">gnda</t>
+    <t xml:space="preserve">vdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memory peripheral supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gnd</t>
   </si>
   <si>
     <t xml:space="preserve">ground</t>
   </si>
   <si>
-    <t xml:space="preserve">vdd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">memory peripheral supply</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gnd</t>
+    <t xml:space="preserve">common ground</t>
   </si>
   <si>
     <t xml:space="preserve">raddr</t>
@@ -215,10 +215,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B6:H20"/>
+  <dimension ref="B6:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -273,13 +273,16 @@
         <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,7 +290,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>9</v>
@@ -296,139 +299,125 @@
         <v>9</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>9</v>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="0" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="0" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
implemented x and y position extraction for pins in the macro excel sheet extractor
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -193,9 +193,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -218,14 +222,15 @@
   <dimension ref="B6:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,10 +246,10 @@
       <c r="E6" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -264,6 +269,13 @@
       <c r="E8" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">10</f>
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>10</v>
+      </c>
       <c r="H8" s="0" t="s">
         <v>10</v>
       </c>
@@ -281,6 +293,14 @@
       <c r="E9" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">F8+10</f>
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H9" s="0" t="s">
         <v>12</v>
       </c>
@@ -298,8 +318,22 @@
       <c r="E10" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">F9+10</f>
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H10" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="1" t="n">
+        <f aca="false">F10+10</f>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -315,6 +349,14 @@
       <c r="E12" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F12" s="1" t="n">
+        <f aca="false">F11+10</f>
+        <v>50</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H12" s="0" t="s">
         <v>18</v>
       </c>
@@ -332,6 +374,14 @@
       <c r="E13" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">F12+10</f>
+        <v>60</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H13" s="0" t="s">
         <v>21</v>
       </c>
@@ -349,8 +399,22 @@
       <c r="E14" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F14" s="1" t="n">
+        <f aca="false">F13+10</f>
+        <v>70</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H14" s="0" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="1" t="n">
+        <f aca="false">F14+10</f>
+        <v>80</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,6 +430,14 @@
       <c r="E16" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">F15+10</f>
+        <v>90</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H16" s="0" t="s">
         <v>26</v>
       </c>
@@ -383,6 +455,14 @@
       <c r="E17" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">F16+10</f>
+        <v>100</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H17" s="0" t="s">
         <v>28</v>
       </c>
@@ -400,6 +480,14 @@
       <c r="E18" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17+10</f>
+        <v>110</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
+      </c>
       <c r="H18" s="0" t="s">
         <v>30</v>
       </c>
@@ -416,6 +504,14 @@
       </c>
       <c r="E19" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18+10</f>
+        <v>120</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <f aca="false">$G$8</f>
+        <v>10</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
implemented analog input signal type
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MEM1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ADC_100MS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -119,6 +120,42 @@
   </si>
   <si>
     <t xml:space="preserve">write clock input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analog supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gnda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">analog ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vddd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital supply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gndd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v_in1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ana_in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input voltage 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v_in2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input voltage 2</t>
   </si>
 </sst>
 </file>
@@ -221,8 +258,8 @@
   </sheetPr>
   <dimension ref="B6:H19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -526,4 +563,211 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.39"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">F7</f>
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <f aca="false">G7+10</f>
+        <v>20</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">F8</f>
+        <v>5</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <f aca="false">G8+10</f>
+        <v>30</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">F9</f>
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <f aca="false">G9+10</f>
+        <v>40</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">F12+10</f>
+        <v>30</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added width and height spec
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t xml:space="preserve">write clock input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">height</t>
   </si>
   <si>
     <t xml:space="preserve">analog supply</t>
@@ -570,10 +576,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -589,176 +595,192 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="H7" s="0" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
         <v>33</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">F7</f>
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <f aca="false">G7+10</f>
-        <v>20</v>
-      </c>
       <c r="H8" s="0" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="1" t="n">
-        <f aca="false">F8</f>
-        <v>5</v>
-      </c>
-      <c r="G9" s="1" t="n">
-        <f aca="false">G8+10</f>
-        <v>30</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>37</v>
-      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <f aca="false">F9</f>
+      <c r="D11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">F10</f>
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="n">
-        <f aca="false">G9+10</f>
-        <v>40</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>39</v>
+      <c r="G11" s="1" t="n">
+        <f aca="false">G10+10</f>
+        <v>20</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="n">
-        <v>20</v>
+        <f aca="false">F11</f>
+        <v>5</v>
       </c>
       <c r="G12" s="1" t="n">
-        <v>10</v>
+        <f aca="false">G11+10</f>
+        <v>30</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">F12</f>
+        <v>5</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <f aca="false">G12+10</f>
+        <v>40</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D15" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="1" t="n">
-        <f aca="false">F12+10</f>
+      <c r="F15" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">F15+10</f>
         <v>30</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>44</v>
+      <c r="G16" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented macro instance list extraction from macro Excel specification
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -162,6 +162,21 @@
   </si>
   <si>
     <t xml:space="preserve">input voltage 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">macro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mem_i0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEM1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mem_i1</t>
   </si>
 </sst>
 </file>
@@ -202,11 +217,88 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
       <bottom/>
       <diagonal/>
     </border>
@@ -236,12 +328,76 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -576,10 +732,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -612,34 +768,36 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="6"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="0" t="s">
@@ -657,12 +815,12 @@
       <c r="G10" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -682,12 +840,12 @@
         <f aca="false">G10+10</f>
         <v>20</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -707,12 +865,12 @@
         <f aca="false">G11+10</f>
         <v>30</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -732,12 +890,16 @@
         <f aca="false">G12+10</f>
         <v>40</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="7" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6"/>
+      <c r="H14" s="7"/>
+    </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -755,12 +917,12 @@
       <c r="G15" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="0" t="s">
@@ -779,8 +941,59 @@
       <c r="G16" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="7" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" s="15" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="16" t="n">
+        <v>110</v>
+      </c>
+      <c r="E22" s="17" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
spec sheet for macro specifications
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -122,10 +122,28 @@
     <t xml:space="preserve">write clock input</t>
   </si>
   <si>
+    <t xml:space="preserve">macro type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mixed signal</t>
+  </si>
+  <si>
     <t xml:space="preserve">width</t>
   </si>
   <si>
     <t xml:space="preserve">height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.lef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.lib</t>
   </si>
   <si>
     <t xml:space="preserve">analog supply</t>
@@ -328,13 +346,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -732,10 +754,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -751,102 +773,78 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="n">
         <v>500</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="C4" s="2" t="n">
         <v>300</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H10" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G10" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="1" t="n">
-        <f aca="false">F10</f>
-        <v>5</v>
-      </c>
-      <c r="G11" s="1" t="n">
-        <f aca="false">G10+10</f>
-        <v>20</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>8</v>
@@ -858,20 +856,18 @@
         <v>9</v>
       </c>
       <c r="F12" s="1" t="n">
-        <f aca="false">F11</f>
         <v>5</v>
       </c>
       <c r="G12" s="1" t="n">
-        <f aca="false">G11+10</f>
-        <v>30</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6" t="s">
-        <v>40</v>
+      <c r="B13" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -888,111 +884,161 @@
       </c>
       <c r="G13" s="1" t="n">
         <f aca="false">G12+10</f>
+        <v>20</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <f aca="false">F13</f>
+        <v>5</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <f aca="false">G13+10</f>
+        <v>30</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <f aca="false">F14</f>
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <f aca="false">G14+10</f>
         <v>40</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="s">
+      <c r="H15" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="7"/>
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F17" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="G17" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="1" t="n">
-        <f aca="false">F15+10</f>
+      <c r="F18" s="1" t="n">
+        <f aca="false">F17+10</f>
         <v>30</v>
       </c>
-      <c r="G16" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="13" t="s">
+      <c r="G18" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E22" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E21" s="15" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="16" t="n">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E23" s="16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="17" t="n">
         <v>110</v>
       </c>
-      <c r="E22" s="17" t="n">
+      <c r="E24" s="18" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added instance to check instance labeling
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t xml:space="preserve">mem_i1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mem_i2</t>
   </si>
 </sst>
 </file>
@@ -754,10 +757,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1036,10 +1039,24 @@
         <v>56</v>
       </c>
       <c r="D24" s="17" t="n">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="E24" s="18" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed related ground generation
</commit_message>
<xml_diff>
--- a/spec/macros.xlsx
+++ b/spec/macros.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
   <si>
     <t xml:space="preserve">pin</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t xml:space="preserve">input voltage 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digital clock</t>
   </si>
   <si>
     <t xml:space="preserve">instance</t>
@@ -757,10 +763,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -995,67 +1001,91 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12" t="s">
+      <c r="B19" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <f aca="false">F18+10</f>
+        <v>40</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="14" t="s">
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E23" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E23" s="16" t="n">
-        <v>10</v>
-      </c>
-    </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="17" t="n">
+      <c r="C24" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="E24" s="16" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="17" t="n">
         <v>210</v>
       </c>
-      <c r="E24" s="18" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="E25" s="18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="1" t="n">
+      <c r="D26" s="1" t="n">
         <v>210</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E26" s="1" t="n">
         <v>160</v>
       </c>
     </row>

</xml_diff>